<commit_message>
[Feature] CIP DO Report Feature Complete. Customized Header
</commit_message>
<xml_diff>
--- a/Reports/IEC Report DO_Report_Iteration_6.xlsx
+++ b/Reports/IEC Report DO_Report_Iteration_6.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="634">
   <si>
     <t>Regression thread</t>
   </si>
@@ -1959,6 +1959,24 @@
     <t>v1_State</t>
   </si>
   <si>
+    <t>v2_label(3)</t>
+  </si>
+  <si>
+    <t>v2_Severity</t>
+  </si>
+  <si>
+    <t>v2_State</t>
+  </si>
+  <si>
+    <t>v3_label(4)</t>
+  </si>
+  <si>
+    <t>v3_Severity</t>
+  </si>
+  <si>
+    <t>v3_State</t>
+  </si>
+  <si>
     <t>15001</t>
   </si>
   <si>
@@ -1968,13 +1986,13 @@
     <t>DO</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Link to Raw Result</t>
   </si>
   <si>
     <t>G08_</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>LF__</t>
@@ -2332,7 +2350,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="62">
+  <fills count="64">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2697,6 +2715,16 @@
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="23"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="23"/>
       </patternFill>
     </fill>
   </fills>
@@ -3438,7 +3466,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="264">
+  <cellXfs count="292">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="24" fontId="25" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="10" fillId="28" fontId="27" numFmtId="0" xfId="0">
@@ -4161,6 +4189,90 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -6456,7 +6568,7 @@
         <v>STD ID</v>
       </c>
       <c r="E3" s="175" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="F3" s="149"/>
       <c r="G3" s="157" t="str">
@@ -6464,7 +6576,7 @@
         <v>Written by</v>
       </c>
       <c r="H3" s="185" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="I3" s="138"/>
       <c r="J3" s="139"/>
@@ -6770,7 +6882,7 @@
         <v>IO schedule version</v>
       </c>
       <c r="E20" t="s" s="184">
-        <v>627</v>
+        <v>633</v>
       </c>
       <c r="F20" s="149"/>
       <c r="G20" s="149"/>
@@ -8215,7 +8327,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -8264,223 +8376,241 @@
         <v>599</v>
       </c>
       <c r="M1" t="s" s="193">
+        <v>600</v>
+      </c>
+      <c r="N1" t="s" s="193">
+        <v>601</v>
+      </c>
+      <c r="O1" t="s" s="193">
+        <v>602</v>
+      </c>
+      <c r="P1" t="s" s="193">
+        <v>603</v>
+      </c>
+      <c r="Q1" t="s" s="193">
+        <v>604</v>
+      </c>
+      <c r="R1" t="s" s="193">
+        <v>605</v>
+      </c>
+      <c r="S1" t="s" s="193">
         <v>586</v>
       </c>
-      <c r="N1" t="s" s="193">
+      <c r="T1" t="s" s="193">
         <v>587</v>
       </c>
-      <c r="O1" t="s" s="194">
+      <c r="U1" t="s" s="194">
         <v>354</v>
       </c>
-      <c r="P1" t="s" s="194">
+      <c r="V1" t="s" s="194">
         <v>356</v>
       </c>
-      <c r="Q1" t="s" s="194">
+      <c r="W1" t="s" s="194">
         <v>20</v>
       </c>
-      <c r="R1" t="s" s="194">
+      <c r="X1" t="s" s="194">
         <v>264</v>
       </c>
-      <c r="S1" t="s" s="194">
+      <c r="Y1" t="s" s="194">
         <v>162</v>
       </c>
-      <c r="T1" t="s" s="194">
+      <c r="Z1" t="s" s="194">
         <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="B2" t="s">
+        <v>612</v>
+      </c>
+      <c r="C2" t="s">
+        <v>614</v>
+      </c>
+      <c r="D2" t="s">
+        <v>613</v>
+      </c>
+      <c r="E2" t="s">
+        <v>615</v>
+      </c>
+      <c r="F2" t="s">
+        <v>608</v>
+      </c>
+      <c r="G2" t="s">
+        <v>616</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" t="s">
         <v>606</v>
       </c>
-      <c r="C2" t="s">
-        <v>608</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="T2" t="s">
         <v>607</v>
       </c>
-      <c r="E2" t="s">
+      <c r="U2" t="s" s="196">
+        <v>22</v>
+      </c>
+      <c r="V2" s="197"/>
+      <c r="W2" s="197" t="s">
         <v>609</v>
       </c>
-      <c r="F2" t="s">
-        <v>602</v>
-      </c>
-      <c r="J2" t="s">
-        <v>610</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>600</v>
-      </c>
-      <c r="N2" t="s">
-        <v>601</v>
-      </c>
-      <c r="O2" t="s" s="196">
-        <v>22</v>
-      </c>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="197" t="s">
-        <v>604</v>
-      </c>
-      <c r="R2" s="197"/>
-      <c r="S2" t="s" s="197">
+      <c r="X2" s="197"/>
+      <c r="Y2" t="s" s="197">
         <v>589</v>
       </c>
-      <c r="T2" t="s" s="197">
+      <c r="Z2" t="s" s="197">
         <v>577</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="B3" t="s">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="C3" t="s">
+        <v>614</v>
+      </c>
+      <c r="D3" t="s">
+        <v>613</v>
+      </c>
+      <c r="E3" t="s">
+        <v>618</v>
+      </c>
+      <c r="F3" t="s">
         <v>608</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
+        <v>616</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" t="s">
+        <v>617</v>
+      </c>
+      <c r="T3" t="s">
         <v>607</v>
       </c>
-      <c r="E3" t="s">
-        <v>612</v>
-      </c>
-      <c r="F3" t="s">
-        <v>602</v>
-      </c>
-      <c r="J3" t="s">
-        <v>610</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" t="s">
-        <v>611</v>
-      </c>
-      <c r="N3" t="s">
-        <v>601</v>
-      </c>
-      <c r="O3" t="s" s="196">
+      <c r="U3" t="s" s="196">
         <v>22</v>
       </c>
-      <c r="P3" s="197"/>
-      <c r="Q3" s="197" t="s">
-        <v>604</v>
-      </c>
-      <c r="R3" s="197"/>
-      <c r="S3" t="s" s="197">
+      <c r="V3" s="197"/>
+      <c r="W3" s="197" t="s">
+        <v>609</v>
+      </c>
+      <c r="X3" s="197"/>
+      <c r="Y3" t="s" s="197">
         <v>589</v>
       </c>
-      <c r="T3" t="s" s="197">
+      <c r="Z3" t="s" s="197">
         <v>577</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="B4" t="s">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="C4" t="s">
+        <v>614</v>
+      </c>
+      <c r="D4" t="s">
+        <v>613</v>
+      </c>
+      <c r="E4" t="s">
+        <v>620</v>
+      </c>
+      <c r="F4" t="s">
         <v>608</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
+        <v>616</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" t="s">
+        <v>619</v>
+      </c>
+      <c r="T4" t="s">
         <v>607</v>
       </c>
-      <c r="E4" t="s">
-        <v>614</v>
-      </c>
-      <c r="F4" t="s">
-        <v>602</v>
-      </c>
-      <c r="J4" t="s">
-        <v>610</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" t="s">
-        <v>613</v>
-      </c>
-      <c r="N4" t="s">
-        <v>601</v>
-      </c>
-      <c r="O4" t="s" s="196">
+      <c r="U4" t="s" s="196">
         <v>22</v>
       </c>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="197" t="s">
-        <v>604</v>
-      </c>
-      <c r="R4" s="197"/>
-      <c r="S4" t="s" s="197">
+      <c r="V4" s="197"/>
+      <c r="W4" s="197" t="s">
+        <v>609</v>
+      </c>
+      <c r="X4" s="197"/>
+      <c r="Y4" t="s" s="197">
         <v>589</v>
       </c>
-      <c r="T4" t="s" s="197">
+      <c r="Z4" t="s" s="197">
         <v>577</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="B5" t="s">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="C5" t="s">
+        <v>614</v>
+      </c>
+      <c r="D5" t="s">
+        <v>613</v>
+      </c>
+      <c r="E5" t="s">
+        <v>622</v>
+      </c>
+      <c r="F5" t="s">
         <v>608</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
+        <v>616</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5" t="s">
+        <v>621</v>
+      </c>
+      <c r="T5" t="s">
         <v>607</v>
       </c>
-      <c r="E5" t="s">
-        <v>616</v>
-      </c>
-      <c r="F5" t="s">
-        <v>602</v>
-      </c>
-      <c r="J5" t="s">
-        <v>610</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" t="s">
-        <v>615</v>
-      </c>
-      <c r="N5" t="s">
-        <v>601</v>
-      </c>
-      <c r="O5" t="s" s="196">
+      <c r="U5" t="s" s="196">
         <v>22</v>
       </c>
-      <c r="P5" s="197"/>
-      <c r="Q5" s="197" t="s">
-        <v>604</v>
-      </c>
-      <c r="R5" s="197"/>
-      <c r="S5" t="s" s="197">
+      <c r="V5" s="197"/>
+      <c r="W5" s="197" t="s">
+        <v>609</v>
+      </c>
+      <c r="X5" s="197"/>
+      <c r="Y5" t="s" s="197">
         <v>589</v>
       </c>
-      <c r="T5" t="s" s="197">
+      <c r="Z5" t="s" s="197">
         <v>577</v>
       </c>
     </row>
@@ -8511,10 +8641,10 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink location="'Raw Result'!3:3" ref="Q2"/>
-    <hyperlink location="'Raw Result'!5:5" ref="Q3"/>
-    <hyperlink location="'Raw Result'!7:7" ref="Q4"/>
-    <hyperlink location="'Raw Result'!9:9" ref="Q5"/>
+    <hyperlink location="'Raw Result'!3:3" ref="W2"/>
+    <hyperlink location="'Raw Result'!5:5" ref="W3"/>
+    <hyperlink location="'Raw Result'!7:7" ref="W4"/>
+    <hyperlink location="'Raw Result'!9:9" ref="W5"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8869,70 +8999,70 @@
       <c r="F1" t="s" s="256">
         <v>595</v>
       </c>
-      <c r="G1" t="s" s="257">
+      <c r="G1" t="s" s="285">
         <v>583</v>
       </c>
-      <c r="I1" t="s" s="258">
-        <v>619</v>
-      </c>
-      <c r="K1" t="s" s="259">
-        <v>620</v>
-      </c>
-      <c r="M1" t="s" s="260">
-        <v>621</v>
-      </c>
-      <c r="O1" t="s" s="261">
-        <v>622</v>
-      </c>
-      <c r="Q1" t="s" s="262">
-        <v>623</v>
-      </c>
-      <c r="S1" t="s" s="263">
-        <v>624</v>
+      <c r="I1" t="s" s="286">
+        <v>625</v>
+      </c>
+      <c r="K1" t="s" s="287">
+        <v>626</v>
+      </c>
+      <c r="M1" t="s" s="288">
+        <v>627</v>
+      </c>
+      <c r="O1" t="s" s="289">
+        <v>628</v>
+      </c>
+      <c r="Q1" t="s" s="290">
+        <v>629</v>
+      </c>
+      <c r="S1" t="s" s="291">
+        <v>630</v>
       </c>
     </row>
     <row r="2">
       <c r="G2" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="H2" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="I2" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="J2" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="K2" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="L2" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="M2" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="N2" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="O2" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="P2" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="Q2" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="R2" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="S2" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="T2" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
     </row>
     <row r="3">
@@ -8945,58 +9075,58 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="D4" t="s">
-        <v>600</v>
+        <v>606</v>
       </c>
       <c r="E4" t="s">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="F4" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="G4" t="s">
-        <v>605</v>
-      </c>
-      <c r="H4" t="s">
-        <v>605</v>
+        <v>610</v>
+      </c>
+      <c r="H4" t="s" s="257">
+        <v>611</v>
       </c>
       <c r="I4" t="s">
-        <v>606</v>
-      </c>
-      <c r="J4" t="s">
-        <v>606</v>
+        <v>612</v>
+      </c>
+      <c r="J4" t="s" s="258">
+        <v>611</v>
       </c>
       <c r="K4" t="s">
+        <v>613</v>
+      </c>
+      <c r="L4" t="s" s="259">
+        <v>611</v>
+      </c>
+      <c r="M4" t="s">
+        <v>614</v>
+      </c>
+      <c r="N4" t="s" s="260">
+        <v>611</v>
+      </c>
+      <c r="O4" t="s">
+        <v>615</v>
+      </c>
+      <c r="P4" t="s" s="261">
+        <v>611</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>616</v>
+      </c>
+      <c r="R4" t="s" s="262">
+        <v>611</v>
+      </c>
+      <c r="S4" t="s">
         <v>607</v>
       </c>
-      <c r="L4" t="s">
-        <v>607</v>
-      </c>
-      <c r="M4" t="s">
-        <v>608</v>
-      </c>
-      <c r="N4" t="s">
-        <v>608</v>
-      </c>
-      <c r="O4" t="s">
-        <v>609</v>
-      </c>
-      <c r="P4" t="s">
-        <v>609</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>610</v>
-      </c>
-      <c r="R4" t="s">
-        <v>610</v>
-      </c>
-      <c r="S4" t="s">
-        <v>601</v>
-      </c>
-      <c r="T4" t="s">
-        <v>601</v>
+      <c r="T4" t="s" s="263">
+        <v>611</v>
       </c>
     </row>
     <row r="5">
@@ -9009,58 +9139,58 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="D6" t="s">
+        <v>617</v>
+      </c>
+      <c r="E6" t="s">
+        <v>607</v>
+      </c>
+      <c r="F6" t="s">
+        <v>607</v>
+      </c>
+      <c r="G6" t="s">
+        <v>610</v>
+      </c>
+      <c r="H6" t="s" s="264">
         <v>611</v>
       </c>
-      <c r="E6" t="s">
-        <v>601</v>
-      </c>
-      <c r="F6" t="s">
-        <v>603</v>
-      </c>
-      <c r="G6" t="s">
-        <v>605</v>
-      </c>
-      <c r="H6" t="s">
-        <v>605</v>
-      </c>
       <c r="I6" t="s">
-        <v>606</v>
-      </c>
-      <c r="J6" t="s">
-        <v>606</v>
+        <v>612</v>
+      </c>
+      <c r="J6" t="s" s="265">
+        <v>611</v>
       </c>
       <c r="K6" t="s">
+        <v>613</v>
+      </c>
+      <c r="L6" t="s" s="266">
+        <v>611</v>
+      </c>
+      <c r="M6" t="s">
+        <v>614</v>
+      </c>
+      <c r="N6" t="s" s="267">
+        <v>611</v>
+      </c>
+      <c r="O6" t="s">
+        <v>618</v>
+      </c>
+      <c r="P6" t="s" s="268">
+        <v>611</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>616</v>
+      </c>
+      <c r="R6" t="s" s="269">
+        <v>611</v>
+      </c>
+      <c r="S6" t="s">
         <v>607</v>
       </c>
-      <c r="L6" t="s">
-        <v>607</v>
-      </c>
-      <c r="M6" t="s">
-        <v>608</v>
-      </c>
-      <c r="N6" t="s">
-        <v>608</v>
-      </c>
-      <c r="O6" t="s">
-        <v>612</v>
-      </c>
-      <c r="P6" t="s">
-        <v>612</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>610</v>
-      </c>
-      <c r="R6" t="s">
-        <v>610</v>
-      </c>
-      <c r="S6" t="s">
-        <v>601</v>
-      </c>
-      <c r="T6" t="s">
-        <v>601</v>
+      <c r="T6" t="s" s="270">
+        <v>611</v>
       </c>
     </row>
     <row r="7">
@@ -9073,58 +9203,58 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="D8" t="s">
+        <v>619</v>
+      </c>
+      <c r="E8" t="s">
+        <v>607</v>
+      </c>
+      <c r="F8" t="s">
+        <v>607</v>
+      </c>
+      <c r="G8" t="s">
+        <v>610</v>
+      </c>
+      <c r="H8" t="s" s="271">
+        <v>611</v>
+      </c>
+      <c r="I8" t="s">
+        <v>612</v>
+      </c>
+      <c r="J8" t="s" s="272">
+        <v>611</v>
+      </c>
+      <c r="K8" t="s">
         <v>613</v>
       </c>
-      <c r="E8" t="s">
-        <v>601</v>
-      </c>
-      <c r="F8" t="s">
-        <v>603</v>
-      </c>
-      <c r="G8" t="s">
-        <v>605</v>
-      </c>
-      <c r="H8" t="s">
-        <v>605</v>
-      </c>
-      <c r="I8" t="s">
-        <v>606</v>
-      </c>
-      <c r="J8" t="s">
-        <v>606</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s" s="273">
+        <v>611</v>
+      </c>
+      <c r="M8" t="s">
+        <v>614</v>
+      </c>
+      <c r="N8" t="s" s="274">
+        <v>611</v>
+      </c>
+      <c r="O8" t="s">
+        <v>620</v>
+      </c>
+      <c r="P8" t="s" s="275">
+        <v>611</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>616</v>
+      </c>
+      <c r="R8" t="s" s="276">
+        <v>611</v>
+      </c>
+      <c r="S8" t="s">
         <v>607</v>
       </c>
-      <c r="L8" t="s">
-        <v>607</v>
-      </c>
-      <c r="M8" t="s">
-        <v>608</v>
-      </c>
-      <c r="N8" t="s">
-        <v>608</v>
-      </c>
-      <c r="O8" t="s">
-        <v>614</v>
-      </c>
-      <c r="P8" t="s">
-        <v>614</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>610</v>
-      </c>
-      <c r="R8" t="s">
-        <v>610</v>
-      </c>
-      <c r="S8" t="s">
-        <v>601</v>
-      </c>
-      <c r="T8" t="s">
-        <v>601</v>
+      <c r="T8" t="s" s="277">
+        <v>611</v>
       </c>
     </row>
     <row r="9">
@@ -9137,58 +9267,58 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="D10" t="s">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="E10" t="s">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="F10" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="G10" t="s">
-        <v>605</v>
-      </c>
-      <c r="H10" t="s">
-        <v>605</v>
+        <v>610</v>
+      </c>
+      <c r="H10" t="s" s="278">
+        <v>611</v>
       </c>
       <c r="I10" t="s">
-        <v>606</v>
-      </c>
-      <c r="J10" t="s">
-        <v>606</v>
+        <v>612</v>
+      </c>
+      <c r="J10" t="s" s="279">
+        <v>611</v>
       </c>
       <c r="K10" t="s">
+        <v>613</v>
+      </c>
+      <c r="L10" t="s" s="280">
+        <v>611</v>
+      </c>
+      <c r="M10" t="s">
+        <v>614</v>
+      </c>
+      <c r="N10" t="s" s="281">
+        <v>611</v>
+      </c>
+      <c r="O10" t="s">
+        <v>622</v>
+      </c>
+      <c r="P10" t="s" s="282">
+        <v>611</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>616</v>
+      </c>
+      <c r="R10" t="s" s="283">
+        <v>611</v>
+      </c>
+      <c r="S10" t="s">
         <v>607</v>
       </c>
-      <c r="L10" t="s">
-        <v>607</v>
-      </c>
-      <c r="M10" t="s">
-        <v>608</v>
-      </c>
-      <c r="N10" t="s">
-        <v>608</v>
-      </c>
-      <c r="O10" t="s">
-        <v>616</v>
-      </c>
-      <c r="P10" t="s">
-        <v>616</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>610</v>
-      </c>
-      <c r="R10" t="s">
-        <v>610</v>
-      </c>
-      <c r="S10" t="s">
-        <v>601</v>
-      </c>
-      <c r="T10" t="s">
-        <v>601</v>
+      <c r="T10" t="s" s="284">
+        <v>611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feature] DO2 Test Report Complete Support
Signed-off-by: Bill Chan <billpwchan@hotmail.com>
</commit_message>
<xml_diff>
--- a/Reports/IEC Report DO_Report_Iteration_6.xlsx
+++ b/Reports/IEC Report DO_Report_Iteration_6.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="634">
   <si>
     <t>Regression thread</t>
   </si>
@@ -8440,8 +8440,8 @@
       <c r="G2" t="s">
         <v>616</v>
       </c>
-      <c r="H2" t="n">
-        <v>0.0</v>
+      <c r="H2" t="s">
+        <v>607</v>
       </c>
       <c r="I2" t="s">
         <v>27</v>
@@ -8489,8 +8489,8 @@
       <c r="G3" t="s">
         <v>616</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.0</v>
+      <c r="H3" t="s">
+        <v>607</v>
       </c>
       <c r="I3" t="s">
         <v>27</v>
@@ -8538,8 +8538,8 @@
       <c r="G4" t="s">
         <v>616</v>
       </c>
-      <c r="H4" t="n">
-        <v>0.0</v>
+      <c r="H4" t="s">
+        <v>607</v>
       </c>
       <c r="I4" t="s">
         <v>27</v>
@@ -8587,8 +8587,8 @@
       <c r="G5" t="s">
         <v>616</v>
       </c>
-      <c r="H5" t="n">
-        <v>0.0</v>
+      <c r="H5" t="s">
+        <v>607</v>
       </c>
       <c r="I5" t="s">
         <v>27</v>

</xml_diff>